<commit_message>
Update project_file from dashboard
</commit_message>
<xml_diff>
--- a/data/Data_project_monitoring.xlsx
+++ b/data/Data_project_monitoring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75DCD77F-03FB-8B4C-B986-AFF5A65CA4CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BACE7A-A17E-514E-AD0B-A0585E964A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{A726FFC7-8C86-2D49-B379-B0BC013886F5}"/>
   </bookViews>
@@ -22,7 +22,7 @@
     <definedName name="vertex42_id" hidden="1">"project-task-list-with-gantt-chart.xlsx"</definedName>
     <definedName name="vertex42_title" hidden="1">"Project Task List with Gantt Chart"</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -762,6 +762,36 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="27">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1482,36 +1512,6 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1526,44 +1526,44 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{38D72556-B332-B44D-ABF6-9BB13F97707D}" name="Table1" displayName="Table1" ref="A1:U127" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" tableBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{38D72556-B332-B44D-ABF6-9BB13F97707D}" name="Table1" displayName="Table1" ref="A1:U127" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25" tableBorderDxfId="24">
   <autoFilter ref="A1:U127" xr:uid="{EA8E0BFA-7E16-439B-A6A0-85575A1D2FBB}"/>
   <tableColumns count="21">
-    <tableColumn id="1" xr3:uid="{9D02E79B-98C3-9844-B380-B0D65AD9DC79}" name="NO" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{5A828F6E-EFF8-CE46-81AF-EF84E7FBA714}" name="KONTRAK" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{CE4724D1-D5E7-CB4A-A5EB-6E18DA13A6AA}" name="NOMOR DOKUMEN &amp; NO. KONTRAK" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{31BCBA83-6CF1-EA4C-8114-585D2F05F082}" name="JENIS PEKERJAAN" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{CB15F02B-1AE6-5140-AABE-09ADE7EFE5D0}" name="AREA PEKERJAAN" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{B96BDF9A-7437-284D-9C86-1C85FE070F2C}" name="SUB AREA PEKERJAAN" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{67B7B1F2-DA8D-9B46-8755-67C5DD3D51A1}" name="CONCATE PEKERJAAN" dataDxfId="14">
+    <tableColumn id="1" xr3:uid="{9D02E79B-98C3-9844-B380-B0D65AD9DC79}" name="NO" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{5A828F6E-EFF8-CE46-81AF-EF84E7FBA714}" name="KONTRAK" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{CE4724D1-D5E7-CB4A-A5EB-6E18DA13A6AA}" name="NOMOR DOKUMEN &amp; NO. KONTRAK" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{31BCBA83-6CF1-EA4C-8114-585D2F05F082}" name="JENIS PEKERJAAN" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{CB15F02B-1AE6-5140-AABE-09ADE7EFE5D0}" name="AREA PEKERJAAN" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{B96BDF9A-7437-284D-9C86-1C85FE070F2C}" name="SUB AREA PEKERJAAN" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{67B7B1F2-DA8D-9B46-8755-67C5DD3D51A1}" name="CONCATE PEKERJAAN" dataDxfId="17">
       <calculatedColumnFormula>B2&amp;D2&amp;F2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{18B6CDE1-CEB3-9E42-8DB1-40EF04ED709D}" name="PRIORITY" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{34E41527-6A3F-2D44-AB92-6C72689B6E9F}" name="START" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{A3FAC971-1E59-A444-B82F-71358E0887BD}" name="PLAN END" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{9079756F-7D3E-0E43-B2A5-5356D486ED21}" name="ACTUAL END" dataDxfId="10"/>
-    <tableColumn id="12" xr3:uid="{945A0098-9CC3-4047-B4F7-CC39A1E31EF5}" name="% COMPLETE" dataDxfId="9" dataCellStyle="Percent"/>
-    <tableColumn id="13" xr3:uid="{AC9C7C90-8B8D-3C45-AE98-E7CFDD3DD916}" name="STATUS" dataDxfId="8"/>
-    <tableColumn id="14" xr3:uid="{50DCA361-CA43-9E4B-8580-927184E6D83C}" name="Project Start" dataDxfId="7"/>
-    <tableColumn id="15" xr3:uid="{0E7BD8A1-5B60-9D47-A4BA-748B04FA60D3}" name="Days to Start" dataDxfId="6">
+    <tableColumn id="8" xr3:uid="{18B6CDE1-CEB3-9E42-8DB1-40EF04ED709D}" name="PRIORITY" dataDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{34E41527-6A3F-2D44-AB92-6C72689B6E9F}" name="START" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{A3FAC971-1E59-A444-B82F-71358E0887BD}" name="PLAN END" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{9079756F-7D3E-0E43-B2A5-5356D486ED21}" name="ACTUAL END" dataDxfId="13"/>
+    <tableColumn id="12" xr3:uid="{945A0098-9CC3-4047-B4F7-CC39A1E31EF5}" name="% COMPLETE" dataDxfId="12" dataCellStyle="Percent"/>
+    <tableColumn id="13" xr3:uid="{AC9C7C90-8B8D-3C45-AE98-E7CFDD3DD916}" name="STATUS" dataDxfId="11"/>
+    <tableColumn id="14" xr3:uid="{50DCA361-CA43-9E4B-8580-927184E6D83C}" name="Project Start" dataDxfId="10"/>
+    <tableColumn id="15" xr3:uid="{0E7BD8A1-5B60-9D47-A4BA-748B04FA60D3}" name="Days to Start" dataDxfId="9">
       <calculatedColumnFormula>IF(ISBLANK(I2),0,I2-N2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{E6EBF2DA-7929-D743-809F-8B720E058B36}" name="Complete" dataDxfId="5">
+    <tableColumn id="16" xr3:uid="{E6EBF2DA-7929-D743-809F-8B720E058B36}" name="Complete" dataDxfId="8">
       <calculatedColumnFormula>$L2*$S2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{8CE5C077-5BDC-0044-A1BB-90BD835F37E1}" name="Incomplete" dataDxfId="4">
+    <tableColumn id="17" xr3:uid="{8CE5C077-5BDC-0044-A1BB-90BD835F37E1}" name="Incomplete" dataDxfId="7">
       <calculatedColumnFormula>S2-P2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{99A1DC32-521F-C74F-A6F5-C70AFB0DA2F6}" name="Slippage" dataDxfId="3">
+    <tableColumn id="18" xr3:uid="{99A1DC32-521F-C74F-A6F5-C70AFB0DA2F6}" name="Slippage" dataDxfId="6">
       <calculatedColumnFormula>IF(ISBLANK(K2),0,(K2-I2)-S2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{C68D290E-7C46-8E46-9B28-77DE939642C2}" name="Plan Days" dataDxfId="2">
+    <tableColumn id="19" xr3:uid="{C68D290E-7C46-8E46-9B28-77DE939642C2}" name="Plan Days" dataDxfId="5">
       <calculatedColumnFormula>IF(ISBLANK(J2),0,J2-I2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{852061C2-A170-5241-A83B-814807443220}" name="SISA DURASI KONTRAK" dataDxfId="1">
+    <tableColumn id="20" xr3:uid="{852061C2-A170-5241-A83B-814807443220}" name="SISA DURASI KONTRAK" dataDxfId="4">
       <calculatedColumnFormula>ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{2E7C9A09-919D-0A46-8438-938686AA48C9}" name="BOBOT" dataDxfId="0"/>
+    <tableColumn id="21" xr3:uid="{2E7C9A09-919D-0A46-8438-938686AA48C9}" name="BOBOT" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1892,8 +1892,8 @@
   <dimension ref="A1:U127"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L5" sqref="L5"/>
+      <pane xSplit="4" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2052,7 +2052,7 @@
       </c>
       <c r="T2" s="24">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>131</v>
+        <v>96</v>
       </c>
       <c r="U2" s="24">
         <v>3.8286127140760531</v>
@@ -2124,7 +2124,7 @@
       </c>
       <c r="T3" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-244</v>
+        <v>-279</v>
       </c>
       <c r="U3" s="25">
         <v>0</v>
@@ -2196,7 +2196,7 @@
       </c>
       <c r="T4" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-104</v>
+        <v>-139</v>
       </c>
       <c r="U4" s="25">
         <v>1.8586563945729366</v>
@@ -2268,7 +2268,7 @@
       </c>
       <c r="T5" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-76</v>
+        <v>-111</v>
       </c>
       <c r="U5" s="25">
         <v>0.79194964416177871</v>
@@ -2340,7 +2340,7 @@
       </c>
       <c r="T6" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-18</v>
+        <v>-53</v>
       </c>
       <c r="U6" s="25">
         <v>1.8581913281290774</v>
@@ -2412,7 +2412,7 @@
       </c>
       <c r="T7" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>9</v>
+        <v>-27</v>
       </c>
       <c r="U7" s="25">
         <v>0.45069827803129847</v>
@@ -2484,7 +2484,7 @@
       </c>
       <c r="T8" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="U8" s="25">
         <v>6.4714074693689341</v>
@@ -2556,7 +2556,7 @@
       </c>
       <c r="T9" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>9</v>
+        <v>-27</v>
       </c>
       <c r="U9" s="25">
         <v>2.1938359438979802</v>
@@ -2628,7 +2628,7 @@
       </c>
       <c r="T10" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-125</v>
+        <v>-160</v>
       </c>
       <c r="U10" s="25">
         <v>1.4899400056670535</v>
@@ -2700,7 +2700,7 @@
       </c>
       <c r="T11" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="U11" s="25">
         <v>33.058446215526629</v>
@@ -2772,7 +2772,7 @@
       </c>
       <c r="T12" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="U12" s="25">
         <v>1.8989416148357232</v>
@@ -2844,7 +2844,7 @@
       </c>
       <c r="T13" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-69</v>
+        <v>-104</v>
       </c>
       <c r="U13" s="25">
         <v>0.61599151131979568</v>
@@ -2916,7 +2916,7 @@
       </c>
       <c r="T14" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-13</v>
+        <v>-48</v>
       </c>
       <c r="U14" s="25">
         <v>0.42275200889415104</v>
@@ -2988,7 +2988,7 @@
       </c>
       <c r="T15" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-6</v>
+        <v>-41</v>
       </c>
       <c r="U15" s="25">
         <v>5.4312137246679076E-2</v>
@@ -3060,7 +3060,7 @@
       </c>
       <c r="T16" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>16</v>
+        <v>-20</v>
       </c>
       <c r="U16" s="25">
         <v>0.74004960479265314</v>
@@ -3132,7 +3132,7 @@
       </c>
       <c r="T17" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>16</v>
+        <v>-20</v>
       </c>
       <c r="U17" s="25">
         <v>0.17748202368678323</v>
@@ -3204,7 +3204,7 @@
       </c>
       <c r="T18" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-76</v>
+        <v>-111</v>
       </c>
       <c r="U18" s="25">
         <v>3.9250044561777282E-2</v>
@@ -3276,7 +3276,7 @@
       </c>
       <c r="T19" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-76</v>
+        <v>-111</v>
       </c>
       <c r="U19" s="25">
         <v>4.9777015190575383E-2</v>
@@ -3348,7 +3348,7 @@
       </c>
       <c r="T20" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>9</v>
+        <v>-27</v>
       </c>
       <c r="U20" s="25">
         <v>1.9866670170786576</v>
@@ -3420,7 +3420,7 @@
       </c>
       <c r="T21" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="U21" s="25">
         <v>8.0826749208230453</v>
@@ -3492,7 +3492,7 @@
       </c>
       <c r="T22" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="U22" s="25">
         <v>4.8861619889981514E-2</v>
@@ -3564,7 +3564,7 @@
       </c>
       <c r="T23" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-6</v>
+        <v>-41</v>
       </c>
       <c r="U23" s="25">
         <v>0.22890573488117585</v>
@@ -3636,7 +3636,7 @@
       </c>
       <c r="T24" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-13</v>
+        <v>-48</v>
       </c>
       <c r="U24" s="25">
         <v>7.4966605347794035E-2</v>
@@ -3708,7 +3708,7 @@
       </c>
       <c r="T25" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="U25" s="25">
         <v>0.4156489033720388</v>
@@ -3780,7 +3780,7 @@
       </c>
       <c r="T26" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="U26" s="25">
         <v>0.34221449233860612</v>
@@ -3852,7 +3852,7 @@
       </c>
       <c r="T27" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-90</v>
+        <v>-125</v>
       </c>
       <c r="U27" s="25">
         <v>2.0404487343946266E-2</v>
@@ -3924,7 +3924,7 @@
       </c>
       <c r="T28" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-48</v>
+        <v>-83</v>
       </c>
       <c r="U28" s="25">
         <v>2.3371433481226382E-2</v>
@@ -3996,7 +3996,7 @@
       </c>
       <c r="T29" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="U29" s="25">
         <v>2.9187755059895788</v>
@@ -4038,7 +4038,7 @@
         <v>45759</v>
       </c>
       <c r="L30" s="19">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M30" s="20" t="s">
         <v>42</v>
@@ -4052,11 +4052,11 @@
       </c>
       <c r="P30" s="22">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>695</v>
       </c>
       <c r="Q30" s="22">
         <f t="shared" si="3"/>
-        <v>139</v>
+        <v>-556</v>
       </c>
       <c r="R30" s="23">
         <f t="shared" si="4"/>
@@ -4068,7 +4068,7 @@
       </c>
       <c r="T30" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="U30" s="25">
         <v>0.11596582079047627</v>
@@ -4140,7 +4140,7 @@
       </c>
       <c r="T31" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>2</v>
+        <v>-34</v>
       </c>
       <c r="U31" s="25">
         <v>8.1747544717989548E-2</v>
@@ -4212,7 +4212,7 @@
       </c>
       <c r="T32" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-48</v>
+        <v>-83</v>
       </c>
       <c r="U32" s="25">
         <v>4.396791761852549E-2</v>
@@ -4284,7 +4284,7 @@
       </c>
       <c r="T33" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-48</v>
+        <v>-83</v>
       </c>
       <c r="U33" s="25">
         <v>1.2091683970173784E-2</v>
@@ -4356,7 +4356,7 @@
       </c>
       <c r="T34" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-90</v>
+        <v>-125</v>
       </c>
       <c r="U34" s="25">
         <v>2.2129086244257725</v>
@@ -4428,7 +4428,7 @@
       </c>
       <c r="T35" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>16</v>
+        <v>-20</v>
       </c>
       <c r="U35" s="25">
         <v>0.7163956909384217</v>
@@ -4500,7 +4500,7 @@
       </c>
       <c r="T36" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>107</v>
+        <v>72</v>
       </c>
       <c r="U36" s="25">
         <v>2.788276283922893</v>
@@ -4572,7 +4572,7 @@
       </c>
       <c r="T37" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>107</v>
+        <v>72</v>
       </c>
       <c r="U37" s="25">
         <v>0.24445340046690409</v>
@@ -4644,7 +4644,7 @@
       </c>
       <c r="T38" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>9</v>
+        <v>-27</v>
       </c>
       <c r="U38" s="25">
         <v>1.3834064445609398</v>
@@ -4716,7 +4716,7 @@
       </c>
       <c r="T39" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-6</v>
+        <v>-41</v>
       </c>
       <c r="U39" s="25">
         <v>0.39134230671971154</v>
@@ -4788,7 +4788,7 @@
       </c>
       <c r="T40" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="U40" s="25">
         <v>0.10777677087659648</v>
@@ -4860,7 +4860,7 @@
       </c>
       <c r="T41" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="U41" s="25">
         <v>8.2318386059768451E-3</v>
@@ -4932,7 +4932,7 @@
       </c>
       <c r="T42" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>2</v>
+        <v>-34</v>
       </c>
       <c r="U42" s="25">
         <v>6.3041469860199054E-2</v>
@@ -5004,7 +5004,7 @@
       </c>
       <c r="T43" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-48</v>
+        <v>-83</v>
       </c>
       <c r="U43" s="25">
         <v>3.5386814494663736E-2</v>
@@ -5076,7 +5076,7 @@
       </c>
       <c r="T44" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="U44" s="25">
         <v>0.58542108403682003</v>
@@ -5148,7 +5148,7 @@
       </c>
       <c r="T45" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="U45" s="25">
         <v>18.96429322855024</v>
@@ -5220,7 +5220,7 @@
       </c>
       <c r="T46" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-48</v>
+        <v>-83</v>
       </c>
       <c r="U46" s="25">
         <v>2.1882553326908354E-2</v>
@@ -5292,7 +5292,7 @@
       </c>
       <c r="T47" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-76</v>
+        <v>-111</v>
       </c>
       <c r="U47" s="25">
         <v>0.10433791562790558</v>
@@ -5364,7 +5364,7 @@
       </c>
       <c r="T48" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>2</v>
+        <v>-34</v>
       </c>
       <c r="U48" s="25">
         <v>1.6500421520262731</v>
@@ -5436,7 +5436,7 @@
       </c>
       <c r="T49" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="U49" s="25">
         <v>1.4876499045579906E-2</v>
@@ -5508,7 +5508,7 @@
       </c>
       <c r="T50" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="U50" s="25">
         <v>6.7954571404563111E-2</v>
@@ -5580,7 +5580,7 @@
       </c>
       <c r="T51" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-48</v>
+        <v>-83</v>
       </c>
       <c r="U51" s="25">
         <v>0.24341470950651456</v>
@@ -5650,7 +5650,7 @@
       </c>
       <c r="T52" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="U52" s="25">
         <v>0</v>
@@ -5722,7 +5722,7 @@
       </c>
       <c r="T53" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="U53" s="25">
         <v>0</v>
@@ -5794,7 +5794,7 @@
       </c>
       <c r="T54" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="U54" s="25">
         <v>0</v>
@@ -5866,7 +5866,7 @@
       </c>
       <c r="T55" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-45</v>
+        <v>-80</v>
       </c>
       <c r="U55" s="25">
         <v>7.3157389496987042</v>
@@ -5938,7 +5938,7 @@
       </c>
       <c r="T56" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>26</v>
+        <v>-10</v>
       </c>
       <c r="U56" s="25">
         <v>1.2678290518311721</v>
@@ -6010,7 +6010,7 @@
       </c>
       <c r="T57" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-12</v>
+        <v>-47</v>
       </c>
       <c r="U57" s="25">
         <v>0.90362130154493769</v>
@@ -6082,7 +6082,7 @@
       </c>
       <c r="T58" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>19</v>
+        <v>-17</v>
       </c>
       <c r="U58" s="25">
         <v>0.90362130154493769</v>
@@ -6154,7 +6154,7 @@
       </c>
       <c r="T59" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>15</v>
+        <v>-21</v>
       </c>
       <c r="U59" s="25">
         <v>0.90362130154493769</v>
@@ -6226,7 +6226,7 @@
       </c>
       <c r="T60" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-35</v>
+        <v>-70</v>
       </c>
       <c r="U60" s="25">
         <v>1.5818776119585585</v>
@@ -6298,7 +6298,7 @@
       </c>
       <c r="T61" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>5</v>
+        <v>-31</v>
       </c>
       <c r="U61" s="25">
         <v>1.2842274814527748</v>
@@ -6370,7 +6370,7 @@
       </c>
       <c r="T62" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-126</v>
+        <v>-161</v>
       </c>
       <c r="U62" s="25">
         <v>6.1841913050091657</v>
@@ -6442,7 +6442,7 @@
       </c>
       <c r="T63" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="U63" s="25">
         <v>0</v>
@@ -6514,7 +6514,7 @@
       </c>
       <c r="T64" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-8</v>
+        <v>-43</v>
       </c>
       <c r="U64" s="25">
         <v>0.94074024135300072</v>
@@ -6586,7 +6586,7 @@
       </c>
       <c r="T65" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-36</v>
+        <v>-71</v>
       </c>
       <c r="U65" s="25">
         <v>1.2317038245452467</v>
@@ -6658,7 +6658,7 @@
       </c>
       <c r="T66" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-65</v>
+        <v>-100</v>
       </c>
       <c r="U66" s="25">
         <v>4.341217820948339</v>
@@ -6730,7 +6730,7 @@
       </c>
       <c r="T67" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-90</v>
+        <v>-125</v>
       </c>
       <c r="U67" s="25">
         <v>1.2874256064363331E-2</v>
@@ -6802,7 +6802,7 @@
       </c>
       <c r="T68" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>22</v>
+        <v>-14</v>
       </c>
       <c r="U68" s="25">
         <v>0.87755848995820385</v>
@@ -6874,7 +6874,7 @@
       </c>
       <c r="T69" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>14</v>
+        <v>-22</v>
       </c>
       <c r="U69" s="25">
         <v>5.6463899562994637</v>
@@ -6946,7 +6946,7 @@
       </c>
       <c r="T70" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-121</v>
+        <v>-156</v>
       </c>
       <c r="U70" s="25">
         <v>3.3921463524873796</v>
@@ -7018,7 +7018,7 @@
       </c>
       <c r="T71" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-14</v>
+        <v>-49</v>
       </c>
       <c r="U71" s="25">
         <v>1.1565364385446064</v>
@@ -7090,7 +7090,7 @@
       </c>
       <c r="T72" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-116</v>
+        <v>-151</v>
       </c>
       <c r="U72" s="25">
         <v>0.35948495436649136</v>
@@ -7162,7 +7162,7 @@
       </c>
       <c r="T73" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="U73" s="25">
         <v>0</v>
@@ -7234,7 +7234,7 @@
       </c>
       <c r="T74" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="U74" s="25">
         <v>0</v>
@@ -7306,7 +7306,7 @@
       </c>
       <c r="T75" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>16</v>
+        <v>-20</v>
       </c>
       <c r="U75" s="25">
         <v>7.3681118933140155</v>
@@ -7378,7 +7378,7 @@
       </c>
       <c r="T76" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>23</v>
+        <v>-13</v>
       </c>
       <c r="U76" s="25">
         <v>1.9262225609604624</v>
@@ -7450,7 +7450,7 @@
       </c>
       <c r="T77" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="U77" s="25">
         <v>0</v>
@@ -7522,7 +7522,7 @@
       </c>
       <c r="T78" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-28</v>
+        <v>-63</v>
       </c>
       <c r="U78" s="25">
         <v>2.6947696149272917</v>
@@ -7594,7 +7594,7 @@
       </c>
       <c r="T79" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-108</v>
+        <v>-143</v>
       </c>
       <c r="U79" s="25">
         <v>7.1455552805644906</v>
@@ -7666,7 +7666,7 @@
       </c>
       <c r="T80" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-118</v>
+        <v>-153</v>
       </c>
       <c r="U80" s="25">
         <v>2.1250737260073151</v>
@@ -7738,7 +7738,7 @@
       </c>
       <c r="T81" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-153</v>
+        <v>-188</v>
       </c>
       <c r="U81" s="25">
         <v>2.2141421850391501</v>
@@ -7810,7 +7810,7 @@
       </c>
       <c r="T82" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-139</v>
+        <v>-174</v>
       </c>
       <c r="U82" s="25">
         <v>2.1434231234710972</v>
@@ -7882,7 +7882,7 @@
       </c>
       <c r="T83" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="U83" s="25">
         <v>0</v>
@@ -7954,7 +7954,7 @@
       </c>
       <c r="T84" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-428</v>
+        <v>-463</v>
       </c>
       <c r="U84" s="25">
         <v>4.2091892986185098</v>
@@ -8026,7 +8026,7 @@
       </c>
       <c r="T85" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>16</v>
+        <v>-20</v>
       </c>
       <c r="U85" s="25">
         <v>0.67906690555318538</v>
@@ -8098,7 +8098,7 @@
       </c>
       <c r="T86" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-139</v>
+        <v>-174</v>
       </c>
       <c r="U86" s="25">
         <v>0.3705846265159719</v>
@@ -8170,7 +8170,7 @@
       </c>
       <c r="T87" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-76</v>
+        <v>-111</v>
       </c>
       <c r="U87" s="25">
         <v>0.46782862216660642</v>
@@ -8242,7 +8242,7 @@
       </c>
       <c r="T88" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-160</v>
+        <v>-195</v>
       </c>
       <c r="U88" s="25">
         <v>2.1434231234710972</v>
@@ -8314,7 +8314,7 @@
       </c>
       <c r="T89" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="U89" s="25">
         <v>0</v>
@@ -8386,7 +8386,7 @@
       </c>
       <c r="T90" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-69</v>
+        <v>-104</v>
       </c>
       <c r="U90" s="25">
         <v>0.66829826225735345</v>
@@ -8458,7 +8458,7 @@
       </c>
       <c r="T91" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-167</v>
+        <v>-202</v>
       </c>
       <c r="U91" s="25">
         <v>0.45089754003550009</v>
@@ -8530,7 +8530,7 @@
       </c>
       <c r="T92" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-153</v>
+        <v>-188</v>
       </c>
       <c r="U92" s="25">
         <v>0.47544300629915759</v>
@@ -8602,7 +8602,7 @@
       </c>
       <c r="T93" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="U93" s="25">
         <v>0</v>
@@ -8674,7 +8674,7 @@
       </c>
       <c r="T94" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-76</v>
+        <v>-111</v>
       </c>
       <c r="U94" s="25">
         <v>7.4012273158472057</v>
@@ -8746,7 +8746,7 @@
       </c>
       <c r="T95" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="U95" s="25">
         <v>0</v>
@@ -8818,7 +8818,7 @@
       </c>
       <c r="T96" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>16</v>
+        <v>-20</v>
       </c>
       <c r="U96" s="25">
         <v>0.12529658962134113</v>
@@ -8890,7 +8890,7 @@
       </c>
       <c r="T97" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="U97" s="25">
         <v>0</v>
@@ -8962,7 +8962,7 @@
       </c>
       <c r="T98" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-181</v>
+        <v>-216</v>
       </c>
       <c r="U98" s="25">
         <v>0.53563667137898285</v>
@@ -9034,7 +9034,7 @@
       </c>
       <c r="T99" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-27</v>
+        <v>-62</v>
       </c>
       <c r="U99" s="25">
         <v>0.31365570942757215</v>
@@ -9106,7 +9106,7 @@
       </c>
       <c r="T100" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-27</v>
+        <v>-62</v>
       </c>
       <c r="U100" s="25">
         <v>0.1502798023901277</v>
@@ -9178,7 +9178,7 @@
       </c>
       <c r="T101" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="U101" s="25">
         <v>0</v>
@@ -9250,7 +9250,7 @@
       </c>
       <c r="T102" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-69</v>
+        <v>-104</v>
       </c>
       <c r="U102" s="25">
         <v>0.1640586615913901</v>
@@ -9322,7 +9322,7 @@
       </c>
       <c r="T103" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-125</v>
+        <v>-160</v>
       </c>
       <c r="U103" s="25">
         <v>0.1502798023901277</v>
@@ -9394,7 +9394,7 @@
       </c>
       <c r="T104" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="U104" s="25">
         <v>0</v>
@@ -9466,7 +9466,7 @@
       </c>
       <c r="T105" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-47</v>
+        <v>-82</v>
       </c>
       <c r="U105" s="25">
         <v>0.41311075421685678</v>
@@ -9538,7 +9538,7 @@
       </c>
       <c r="T106" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-47</v>
+        <v>-82</v>
       </c>
       <c r="U106" s="25">
         <v>0.41311075421685678</v>
@@ -9610,7 +9610,7 @@
       </c>
       <c r="T107" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="U107" s="25">
         <v>0</v>
@@ -9682,7 +9682,7 @@
       </c>
       <c r="T108" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-6</v>
+        <v>-41</v>
       </c>
       <c r="U108" s="25">
         <v>0.71590581972999912</v>
@@ -9754,7 +9754,7 @@
       </c>
       <c r="T109" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="U109" s="25">
         <v>0</v>
@@ -9826,7 +9826,7 @@
       </c>
       <c r="T110" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="U110" s="25">
         <v>0</v>
@@ -9898,7 +9898,7 @@
       </c>
       <c r="T111" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-6</v>
+        <v>-41</v>
       </c>
       <c r="U111" s="25">
         <v>1.1364470150796924</v>
@@ -9970,7 +9970,7 @@
       </c>
       <c r="T112" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="U112" s="25">
         <v>0</v>
@@ -10042,7 +10042,7 @@
       </c>
       <c r="T113" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-90</v>
+        <v>-125</v>
       </c>
       <c r="U113" s="25">
         <v>0.86888955106354271</v>
@@ -10114,7 +10114,7 @@
       </c>
       <c r="T114" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-75</v>
+        <v>-110</v>
       </c>
       <c r="U114" s="25">
         <v>1.9101722387327178</v>
@@ -10186,7 +10186,7 @@
       </c>
       <c r="T115" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>16</v>
+        <v>-20</v>
       </c>
       <c r="U115" s="25">
         <v>2.3615133681493417</v>
@@ -10258,7 +10258,7 @@
       </c>
       <c r="T116" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="U116" s="25">
         <v>0</v>
@@ -10330,7 +10330,7 @@
       </c>
       <c r="T117" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="U117" s="25">
         <v>0</v>
@@ -10402,7 +10402,7 @@
       </c>
       <c r="T118" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="U118" s="25">
         <v>0</v>
@@ -10474,7 +10474,7 @@
       </c>
       <c r="T119" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-97</v>
+        <v>-132</v>
       </c>
       <c r="U119" s="25">
         <v>1.2772542166873568</v>
@@ -10546,7 +10546,7 @@
       </c>
       <c r="T120" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-27</v>
+        <v>-62</v>
       </c>
       <c r="U120" s="25">
         <v>1.3021928291029847</v>
@@ -10618,7 +10618,7 @@
       </c>
       <c r="T121" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-6</v>
+        <v>-41</v>
       </c>
       <c r="U121" s="25">
         <v>2.2106399922458855</v>
@@ -10690,7 +10690,7 @@
       </c>
       <c r="T122" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-75</v>
+        <v>-110</v>
       </c>
       <c r="U122" s="25">
         <v>0.94089880391742786</v>
@@ -10762,7 +10762,7 @@
       </c>
       <c r="T123" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>2</v>
+        <v>-34</v>
       </c>
       <c r="U123" s="25">
         <v>0.83220228058553414</v>
@@ -10834,7 +10834,7 @@
       </c>
       <c r="T124" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>2</v>
+        <v>-34</v>
       </c>
       <c r="U124" s="25">
         <v>1.1429745636452144</v>
@@ -10906,7 +10906,7 @@
       </c>
       <c r="T125" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-69</v>
+        <v>-104</v>
       </c>
       <c r="U125" s="25">
         <v>0.65729302337862683</v>
@@ -10978,7 +10978,7 @@
       </c>
       <c r="T126" s="25">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>-37</v>
+        <v>-72</v>
       </c>
       <c r="U126" s="25">
         <v>1.1353862689916343</v>
@@ -11050,7 +11050,7 @@
       </c>
       <c r="T127" s="47">
         <f ca="1">ROUNDUP(Table1[[#This Row],[PLAN END]]-NOW(),0)</f>
-        <v>30</v>
+        <v>-6</v>
       </c>
       <c r="U127" s="47">
         <v>0.45616355925610708</v>
@@ -11058,13 +11058,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:H127">
-    <cfRule type="containsText" dxfId="26" priority="5" operator="containsText" text="LOW">
+    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",H2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="6" operator="containsText" text="MEDIUM">
+    <cfRule type="containsText" dxfId="1" priority="6" operator="containsText" text="MEDIUM">
       <formula>NOT(ISERROR(SEARCH("MEDIUM",H2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="7" operator="containsText" text="HIGH">
+    <cfRule type="containsText" dxfId="0" priority="7" operator="containsText" text="HIGH">
       <formula>NOT(ISERROR(SEARCH("HIGH",H2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>